<commit_message>
update including backup function dummy coding
mainly to save first dummy coding function
</commit_message>
<xml_diff>
--- a/data_raw/2024_census/processed/dat_ko_variables_selection_filled.xlsx
+++ b/data_raw/2024_census/processed/dat_ko_variables_selection_filled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzoehler/Documents/GitHub/SAE_WS25/data_raw/2024_census/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE0D249-1F20-EA41-97E9-BBFFD9768E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E61B5D-541B-C54F-B233-1347CB45A664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24000" yWindow="500" windowWidth="14400" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="211">
   <si>
     <t>variable</t>
   </si>
@@ -100,9 +100,6 @@
     <t>p38_asiste</t>
   </si>
   <si>
-    <t>hh_v19c_compu</t>
-  </si>
-  <si>
     <t>p42d_comuni</t>
   </si>
   <si>
@@ -112,177 +109,69 @@
     <t>p42b_oir</t>
   </si>
   <si>
-    <t>hh_v10_combus</t>
-  </si>
-  <si>
     <t>asiste</t>
   </si>
   <si>
-    <t>hh_v06_piso</t>
-  </si>
-  <si>
-    <t>hh_v19e_f</t>
-  </si>
-  <si>
-    <t>hh_v11_basura</t>
-  </si>
-  <si>
     <t>p42_discap</t>
   </si>
   <si>
     <t>p31_afiliado</t>
   </si>
   <si>
-    <t>hh_v19f_inetmovil</t>
-  </si>
-  <si>
-    <t>hh_v19e_inetfijo</t>
-  </si>
-  <si>
     <t>p42a_ver</t>
   </si>
   <si>
-    <t>hh_v03_pared</t>
-  </si>
-  <si>
-    <t>hh_v19b_tv</t>
-  </si>
-  <si>
-    <t>hh_v18j_lavadora</t>
-  </si>
-  <si>
-    <t>hh_urbrur</t>
-  </si>
-  <si>
     <t>p43_pago</t>
   </si>
   <si>
     <t>dep_nac_cod</t>
   </si>
   <si>
-    <t>hh_v18f_refri</t>
-  </si>
-  <si>
-    <t>hh_v15_servsan</t>
-  </si>
-  <si>
-    <t>hh_v19h_d</t>
-  </si>
-  <si>
-    <t>hh_v19d_celular</t>
-  </si>
-  <si>
     <t>p37_lugres5</t>
   </si>
   <si>
-    <t>hh_v19g_tvcable</t>
-  </si>
-  <si>
     <t>p30b_caja</t>
   </si>
   <si>
-    <t>hh_v08_aguadist</t>
-  </si>
-  <si>
-    <t>hh_v18g_micro</t>
-  </si>
-  <si>
-    <t>hh_v17_tenencia</t>
-  </si>
-  <si>
     <t>dep_res_cod</t>
   </si>
   <si>
     <t>idep</t>
   </si>
   <si>
-    <t>hh_idep</t>
-  </si>
-  <si>
     <t>dep_res5_cod</t>
   </si>
   <si>
-    <t>hh_v18c_auto</t>
-  </si>
-  <si>
-    <t>hh_v05_techo</t>
-  </si>
-  <si>
     <t>p32_pueblo_per</t>
   </si>
   <si>
-    <t>hh_v04_revoq</t>
-  </si>
-  <si>
     <t>p35_lugnac</t>
   </si>
   <si>
     <t>p30c_privad</t>
   </si>
   <si>
-    <t>hh_tip_hog</t>
-  </si>
-  <si>
-    <t>hh_v07_aguapro</t>
-  </si>
-  <si>
     <t>condact_19</t>
   </si>
   <si>
-    <t>hh_v14_dormit</t>
-  </si>
-  <si>
-    <t>hh_v09_energia</t>
-  </si>
-  <si>
-    <t>hh_v18a_bici</t>
-  </si>
-  <si>
     <t>p25_sexo</t>
   </si>
   <si>
-    <t>hh_v18b_moto</t>
-  </si>
-  <si>
-    <t>hh_v18h_calefon</t>
-  </si>
-  <si>
-    <t>hh_v18i_aire</t>
-  </si>
-  <si>
-    <t>hh_v13_habitac</t>
-  </si>
-  <si>
-    <t>hh_v20a_emi</t>
-  </si>
-  <si>
     <t>p30f_autome</t>
   </si>
   <si>
     <t>p36_lugres</t>
   </si>
   <si>
-    <t>hh_v19a_radio</t>
-  </si>
-  <si>
     <t>p30a_public</t>
   </si>
   <si>
     <t>imun</t>
   </si>
   <si>
-    <t>hh_imun</t>
-  </si>
-  <si>
     <t>p30d_atedom</t>
   </si>
   <si>
-    <t>hh_v19h_telfijo</t>
-  </si>
-  <si>
-    <t>hh_v18d_carreta</t>
-  </si>
-  <si>
     <t>condact_13</t>
   </si>
   <si>
@@ -304,12 +193,6 @@
     <t>pet_19</t>
   </si>
   <si>
-    <t>hh_v12_cocina</t>
-  </si>
-  <si>
-    <t>hh_v18e_bote</t>
-  </si>
-  <si>
     <t>pet_13</t>
   </si>
   <si>
@@ -319,9 +202,6 @@
     <t>p31_cobersalud</t>
   </si>
   <si>
-    <t>hh_v21a_fal</t>
-  </si>
-  <si>
     <t>i00</t>
   </si>
   <si>
@@ -388,24 +268,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>hh_iprov</t>
-  </si>
-  <si>
-    <t>hh_v01_tipoviv</t>
-  </si>
-  <si>
-    <t>hh_v02_condocup</t>
-  </si>
-  <si>
-    <t>hh_tot_pers</t>
-  </si>
-  <si>
-    <t>hh_matchingID</t>
-  </si>
-  <si>
-    <t>hh_ID</t>
-  </si>
-  <si>
     <t>include</t>
   </si>
   <si>
@@ -668,6 +530,129 @@
   </si>
   <si>
     <t xml:space="preserve">Activity status (7 years or older) 13th CIET (job status: employed, jobless, seeking job) </t>
+  </si>
+  <si>
+    <t>v19c_compu</t>
+  </si>
+  <si>
+    <t>v10_combus</t>
+  </si>
+  <si>
+    <t>v06_piso</t>
+  </si>
+  <si>
+    <t>v19e_f</t>
+  </si>
+  <si>
+    <t>v11_basura</t>
+  </si>
+  <si>
+    <t>v19f_inetmovil</t>
+  </si>
+  <si>
+    <t>v19e_inetfijo</t>
+  </si>
+  <si>
+    <t>v03_pared</t>
+  </si>
+  <si>
+    <t>v19b_tv</t>
+  </si>
+  <si>
+    <t>v18j_lavadora</t>
+  </si>
+  <si>
+    <t>urbrur</t>
+  </si>
+  <si>
+    <t>v18f_refri</t>
+  </si>
+  <si>
+    <t>v15_servsan</t>
+  </si>
+  <si>
+    <t>v19h_d</t>
+  </si>
+  <si>
+    <t>v19d_celular</t>
+  </si>
+  <si>
+    <t>v19g_tvcable</t>
+  </si>
+  <si>
+    <t>v08_aguadist</t>
+  </si>
+  <si>
+    <t>v18g_micro</t>
+  </si>
+  <si>
+    <t>v17_tenencia</t>
+  </si>
+  <si>
+    <t>v18c_auto</t>
+  </si>
+  <si>
+    <t>v05_techo</t>
+  </si>
+  <si>
+    <t>v04_revoq</t>
+  </si>
+  <si>
+    <t>tip_hog</t>
+  </si>
+  <si>
+    <t>v07_aguapro</t>
+  </si>
+  <si>
+    <t>v14_dormit</t>
+  </si>
+  <si>
+    <t>v09_energia</t>
+  </si>
+  <si>
+    <t>v18a_bici</t>
+  </si>
+  <si>
+    <t>v18b_moto</t>
+  </si>
+  <si>
+    <t>v18h_calefon</t>
+  </si>
+  <si>
+    <t>v18i_aire</t>
+  </si>
+  <si>
+    <t>v13_habitac</t>
+  </si>
+  <si>
+    <t>v20a_emi</t>
+  </si>
+  <si>
+    <t>v19a_radio</t>
+  </si>
+  <si>
+    <t>v19h_telfijo</t>
+  </si>
+  <si>
+    <t>v18d_carreta</t>
+  </si>
+  <si>
+    <t>v12_cocina</t>
+  </si>
+  <si>
+    <t>v18e_bote</t>
+  </si>
+  <si>
+    <t>v21a_fal</t>
+  </si>
+  <si>
+    <t>v01_tipoviv</t>
+  </si>
+  <si>
+    <t>v02_condocup</t>
+  </si>
+  <si>
+    <t>tot_pers</t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="89" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1093,10 +1078,10 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="O1" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1140,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -1184,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -1228,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -1272,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1316,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -1360,10 +1345,10 @@
         <v>0.21282999999999999</v>
       </c>
       <c r="N7" t="s">
-        <v>210</v>
+        <v>164</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -1407,10 +1392,10 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>133</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -1454,10 +1439,10 @@
         <v>4.2130000000000001E-2</v>
       </c>
       <c r="N9" t="s">
-        <v>210</v>
+        <v>164</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -1501,10 +1486,10 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>210</v>
+        <v>164</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -1548,10 +1533,10 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>210</v>
+        <v>164</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1595,10 +1580,10 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1642,10 +1627,10 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1689,15 +1674,15 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>170</v>
       </c>
       <c r="B15">
         <v>8.0400000000000003E-3</v>
@@ -1736,15 +1721,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N15" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>2.988E-2</v>
@@ -1783,15 +1768,15 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>7.6000000000000004E-4</v>
@@ -1830,15 +1815,15 @@
         <v>0.21282999999999999</v>
       </c>
       <c r="N17" t="s">
-        <v>210</v>
+        <v>164</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>2.7269999999999999E-2</v>
@@ -1877,15 +1862,15 @@
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>171</v>
       </c>
       <c r="B19">
         <v>3.1029999999999999E-2</v>
@@ -1924,15 +1909,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N19" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20">
         <v>6.6780000000000006E-2</v>
@@ -1971,15 +1956,15 @@
         <v>4.2130000000000001E-2</v>
       </c>
       <c r="N20" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="O20" t="s">
-        <v>211</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>172</v>
       </c>
       <c r="B21">
         <v>3.2149999999999998E-2</v>
@@ -2018,15 +2003,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N21" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>173</v>
       </c>
       <c r="B22">
         <v>7.0200000000000002E-3</v>
@@ -2065,15 +2050,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N22" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>174</v>
       </c>
       <c r="B23">
         <v>3.891E-2</v>
@@ -2112,15 +2097,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N23" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>5.3039999999999997E-2</v>
@@ -2159,15 +2144,15 @@
         <v>1.4290000000000001E-2</v>
       </c>
       <c r="N24" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B25">
         <v>3.1900000000000001E-3</v>
@@ -2206,15 +2191,15 @@
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>212</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
       <c r="B26">
         <v>5.7299999999999999E-3</v>
@@ -2253,15 +2238,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N26" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>176</v>
       </c>
       <c r="B27">
         <v>3.7499999999999999E-3</v>
@@ -2300,15 +2285,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N27" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B28">
         <v>2.249E-2</v>
@@ -2347,15 +2332,15 @@
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>177</v>
       </c>
       <c r="B29">
         <v>1.1820000000000001E-2</v>
@@ -2394,15 +2379,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N29" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>178</v>
       </c>
       <c r="B30">
         <v>5.0299999999999997E-3</v>
@@ -2441,15 +2426,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N30" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>179</v>
       </c>
       <c r="B31">
         <v>3.0699999999999998E-3</v>
@@ -2488,15 +2473,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N31" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>180</v>
       </c>
       <c r="B32">
         <v>3.4660000000000003E-2</v>
@@ -2535,15 +2520,15 @@
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>1.106E-2</v>
@@ -2582,15 +2567,15 @@
         <v>0</v>
       </c>
       <c r="N33" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>6.6E-4</v>
@@ -2629,15 +2614,15 @@
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>213</v>
+        <v>167</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
       <c r="B35">
         <v>4.3600000000000002E-3</v>
@@ -2676,15 +2661,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N35" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>182</v>
       </c>
       <c r="B36">
         <v>1.9E-2</v>
@@ -2723,15 +2708,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N36" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>183</v>
       </c>
       <c r="B37">
         <v>2E-3</v>
@@ -2770,15 +2755,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N37" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>184</v>
       </c>
       <c r="B38">
         <v>1.97E-3</v>
@@ -2817,15 +2802,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N38" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B39">
         <v>5.9500000000000004E-3</v>
@@ -2864,15 +2849,15 @@
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>213</v>
+        <v>167</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>214</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="B40">
         <v>2.4599999999999999E-3</v>
@@ -2911,15 +2896,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N40" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B41">
         <v>7.2899999999999996E-3</v>
@@ -2958,12 +2943,12 @@
         <v>0</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>163</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>186</v>
       </c>
       <c r="B42">
         <v>2.3189999999999999E-2</v>
@@ -3002,15 +2987,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N42" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>187</v>
       </c>
       <c r="B43">
         <v>1.57E-3</v>
@@ -3049,15 +3034,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N43" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>188</v>
       </c>
       <c r="B44">
         <v>1.3310000000000001E-2</v>
@@ -3096,15 +3081,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N44" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B45">
         <v>3.8000000000000002E-4</v>
@@ -3143,15 +3128,15 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B46">
         <v>3.63E-3</v>
@@ -3190,15 +3175,15 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B47">
         <v>3.63E-3</v>
@@ -3237,15 +3222,15 @@
         <v>0</v>
       </c>
       <c r="N47" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B48">
         <v>5.5000000000000003E-4</v>
@@ -3284,15 +3269,15 @@
         <v>0</v>
       </c>
       <c r="N48" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>170</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>189</v>
       </c>
       <c r="B49">
         <v>2.7599999999999999E-3</v>
@@ -3331,15 +3316,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N49" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>171</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>190</v>
       </c>
       <c r="B50">
         <v>6.0800000000000003E-3</v>
@@ -3378,15 +3363,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N50" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B51">
         <v>3.0799999999999998E-3</v>
@@ -3425,15 +3410,15 @@
         <v>0</v>
       </c>
       <c r="N51" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>173</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>191</v>
       </c>
       <c r="B52">
         <v>2.0580000000000001E-2</v>
@@ -3472,15 +3457,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N52" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="B53">
         <v>9.6600000000000002E-3</v>
@@ -3519,15 +3504,15 @@
         <v>0</v>
       </c>
       <c r="N53" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B54">
         <v>5.1799999999999997E-3</v>
@@ -3566,15 +3551,15 @@
         <v>0</v>
       </c>
       <c r="N54" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>176</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>192</v>
       </c>
       <c r="B55">
         <v>5.3699999999999998E-3</v>
@@ -3613,12 +3598,12 @@
         <v>2.478E-2</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>177</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="B56">
         <v>9.8799999999999999E-3</v>
@@ -3657,12 +3642,12 @@
         <v>2.478E-2</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>178</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B57">
         <v>1.0580000000000001E-2</v>
@@ -3701,12 +3686,12 @@
         <v>0</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>179</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>194</v>
       </c>
       <c r="B58">
         <v>1.0580000000000001E-2</v>
@@ -3745,12 +3730,12 @@
         <v>2.478E-2</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>180</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>195</v>
       </c>
       <c r="B59">
         <v>1.438E-2</v>
@@ -3789,12 +3774,12 @@
         <v>2.478E-2</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>181</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>196</v>
       </c>
       <c r="B60">
         <v>2.2499999999999998E-3</v>
@@ -3833,12 +3818,12 @@
         <v>2.478E-2</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>182</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B61">
         <v>1.1509999999999999E-2</v>
@@ -3877,15 +3862,15 @@
         <v>0</v>
       </c>
       <c r="N61" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>197</v>
       </c>
       <c r="B62">
         <v>1.6900000000000001E-3</v>
@@ -3924,15 +3909,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N62" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>184</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>198</v>
       </c>
       <c r="B63">
         <v>5.6999999999999998E-4</v>
@@ -3971,15 +3956,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N63" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>199</v>
       </c>
       <c r="B64">
         <v>5.1999999999999995E-4</v>
@@ -4018,15 +4003,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N64" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>186</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>200</v>
       </c>
       <c r="B65">
         <v>3.6600000000000001E-3</v>
@@ -4065,15 +4050,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N65" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>187</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>201</v>
       </c>
       <c r="B66">
         <v>6.4799999999999996E-3</v>
@@ -4112,12 +4097,12 @@
         <v>2.478E-2</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>188</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="B67">
         <v>2.0100000000000001E-3</v>
@@ -4156,12 +4141,12 @@
         <v>0</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>189</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B68">
         <v>5.3099999999999996E-3</v>
@@ -4200,12 +4185,12 @@
         <v>0</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>190</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>202</v>
       </c>
       <c r="B69">
         <v>1.01E-3</v>
@@ -4244,12 +4229,12 @@
         <v>2.478E-2</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>191</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="B70">
         <v>1.82E-3</v>
@@ -4288,15 +4273,15 @@
         <v>0</v>
       </c>
       <c r="N70" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="B71">
         <v>3.6000000000000002E-4</v>
@@ -4335,12 +4320,12 @@
         <v>0</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>193</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B72">
         <v>3.6000000000000002E-4</v>
@@ -4379,12 +4364,12 @@
         <v>0</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>194</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="B73">
         <v>6.8999999999999997E-4</v>
@@ -4423,15 +4408,15 @@
         <v>0</v>
       </c>
       <c r="N73" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O73" s="1" t="s">
-        <v>195</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>85</v>
+        <v>203</v>
       </c>
       <c r="B74">
         <v>3.2000000000000003E-4</v>
@@ -4470,15 +4455,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N74" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O74" s="1" t="s">
-        <v>196</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
       <c r="B75">
         <v>4.0000000000000003E-5</v>
@@ -4517,15 +4502,15 @@
         <v>2.478E-2</v>
       </c>
       <c r="N75" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="O75" s="1" t="s">
-        <v>197</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="B76">
         <v>5.5000000000000003E-4</v>
@@ -4564,15 +4549,15 @@
         <v>0</v>
       </c>
       <c r="N76" t="s">
-        <v>210</v>
+        <v>164</v>
       </c>
       <c r="O76" s="1" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="B77">
         <v>8.0000000000000004E-4</v>
@@ -4611,15 +4596,15 @@
         <v>0.19869000000000001</v>
       </c>
       <c r="N77" t="s">
-        <v>210</v>
+        <v>164</v>
       </c>
       <c r="O77" s="1" t="s">
-        <v>198</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="B78">
         <v>3.8000000000000002E-4</v>
@@ -4658,15 +4643,15 @@
         <v>0</v>
       </c>
       <c r="N78" t="s">
-        <v>213</v>
+        <v>167</v>
       </c>
       <c r="O78" s="1" t="s">
-        <v>199</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="B79">
         <v>1.6000000000000001E-4</v>
@@ -4705,12 +4690,12 @@
         <v>0</v>
       </c>
       <c r="O79" s="1" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="B80">
         <v>3.6999999999999999E-4</v>
@@ -4749,12 +4734,12 @@
         <v>0</v>
       </c>
       <c r="O80" s="1" t="s">
-        <v>201</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="B81">
         <v>2.5000000000000001E-4</v>
@@ -4793,12 +4778,12 @@
         <v>0.29299999999999998</v>
       </c>
       <c r="O81" s="1" t="s">
-        <v>202</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="B82">
         <v>3.5E-4</v>
@@ -4837,12 +4822,12 @@
         <v>0</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>203</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>94</v>
+        <v>205</v>
       </c>
       <c r="B83">
         <v>3.2000000000000003E-4</v>
@@ -4881,12 +4866,12 @@
         <v>2.478E-2</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>95</v>
+        <v>206</v>
       </c>
       <c r="B84">
         <v>1.7000000000000001E-4</v>
@@ -4925,12 +4910,12 @@
         <v>2.478E-2</v>
       </c>
       <c r="O84" s="1" t="s">
-        <v>205</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="B85">
         <v>2.1000000000000001E-4</v>
@@ -4969,12 +4954,12 @@
         <v>0</v>
       </c>
       <c r="O85" s="1" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="B86">
         <v>8.0000000000000007E-5</v>
@@ -5013,12 +4998,12 @@
         <v>0</v>
       </c>
       <c r="O86" s="1" t="s">
-        <v>207</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="B87">
         <v>1.3999999999999999E-4</v>
@@ -5057,12 +5042,12 @@
         <v>1.6619999999999999E-2</v>
       </c>
       <c r="O87" s="1" t="s">
-        <v>208</v>
+        <v>162</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>99</v>
+        <v>207</v>
       </c>
       <c r="B88">
         <v>1.3999999999999999E-4</v>
@@ -5101,12 +5086,12 @@
         <v>2.478E-2</v>
       </c>
       <c r="O88" s="1" t="s">
-        <v>209</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F89">
         <v>6828</v>
@@ -5135,7 +5120,7 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="F90">
         <v>20</v>
@@ -5164,7 +5149,7 @@
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="F91">
         <v>16</v>
@@ -5193,7 +5178,7 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="F92">
         <v>79</v>
@@ -5222,7 +5207,7 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="F93">
         <v>25</v>
@@ -5251,7 +5236,7 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="F94">
         <v>25</v>
@@ -5280,7 +5265,7 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="F95">
         <v>95</v>
@@ -5309,7 +5294,7 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="F96">
         <v>23</v>
@@ -5338,7 +5323,7 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="F97">
         <v>17</v>
@@ -5367,7 +5352,7 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="F98">
         <v>21</v>
@@ -5396,7 +5381,7 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="F99">
         <v>25</v>
@@ -5425,7 +5410,7 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="F100">
         <v>25</v>
@@ -5454,7 +5439,7 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="F101">
         <v>45</v>
@@ -5483,7 +5468,7 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="F102">
         <v>124</v>
@@ -5512,7 +5497,7 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="F103">
         <v>422</v>
@@ -5541,7 +5526,7 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="F104">
         <v>123</v>
@@ -5570,7 +5555,7 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="F105">
         <v>368</v>
@@ -5599,7 +5584,7 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="F106">
         <v>124</v>
@@ -5628,7 +5613,7 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="F107">
         <v>385</v>
@@ -5657,7 +5642,7 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="F108">
         <v>22</v>
@@ -5686,7 +5671,7 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="F109">
         <v>343</v>
@@ -5715,7 +5700,7 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="F110">
         <v>6860</v>
@@ -5729,7 +5714,7 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>122</v>
+        <v>61</v>
       </c>
       <c r="F111">
         <v>20</v>
@@ -5758,7 +5743,7 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>123</v>
+        <v>208</v>
       </c>
       <c r="F112">
         <v>16</v>
@@ -5787,7 +5772,7 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>124</v>
+        <v>209</v>
       </c>
       <c r="F113">
         <v>1</v>
@@ -5816,7 +5801,7 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
       <c r="F114">
         <v>77</v>
@@ -5845,7 +5830,7 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="F115">
         <v>343</v>
@@ -5874,7 +5859,7 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="F116">
         <v>6828</v>

</xml_diff>